<commit_message>
Adding a new function!
</commit_message>
<xml_diff>
--- a/Bus_Booking/Dat_Ve_Xe_Khach.xlsx
+++ b/Bus_Booking/Dat_Ve_Xe_Khach.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Online\Database Management System\TH\Git\Dat_Ve_Xe_Khach\Bus_Booking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2452FFCA-900A-4E28-B186-C3B9C80E2C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7128FC5A-89EC-4F70-A823-617511DC1A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8C09623A-A02A-4DFB-923B-F792C92F998F}"/>
   </bookViews>
@@ -679,7 +679,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -691,19 +691,18 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -715,14 +714,16 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1040,7 +1041,7 @@
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F15" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1076,21 +1077,21 @@
       <c r="L1" s="6"/>
     </row>
     <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="E2" s="10" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="E2" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="I2" s="10" t="s">
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="I2" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
       <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
@@ -1366,21 +1367,21 @@
       <c r="L14" s="6"/>
     </row>
     <row r="15" spans="1:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="E15" s="10" t="s">
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="E15" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="I15" s="14" t="s">
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="I15" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="J15" s="15"/>
-      <c r="K15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="17"/>
       <c r="L15" s="6"/>
     </row>
     <row r="16" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
@@ -1584,21 +1585,21 @@
       <c r="L24" s="6"/>
     </row>
     <row r="25" spans="1:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="E25" s="17" t="s">
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="E25" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="I25" s="17" t="s">
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="I25" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
     </row>
     <row r="26" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
@@ -1610,18 +1611,18 @@
       <c r="C26" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E26" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="I26" s="20" t="s">
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="I26" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="J26" s="20" t="s">
+      <c r="J26" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="K26" s="20" t="s">
+      <c r="K26" s="11" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1635,18 +1636,18 @@
       <c r="C27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="I27" s="18" t="s">
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="I27" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="J27" s="18" t="s">
+      <c r="J27" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="K27" s="18" t="s">
+      <c r="K27" s="9" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1660,18 +1661,18 @@
       <c r="C28" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E28" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="I28" s="18" t="s">
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="I28" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="J28" s="18" t="s">
+      <c r="J28" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="K28" s="18"/>
+      <c r="K28" s="9"/>
     </row>
     <row r="29" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
@@ -1683,18 +1684,18 @@
       <c r="C29" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="I29" s="18" t="s">
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="I29" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="J29" s="18" t="s">
+      <c r="J29" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="K29" s="18"/>
+      <c r="K29" s="9"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
@@ -1706,18 +1707,18 @@
       <c r="C30" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="I30" s="18" t="s">
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="I30" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="J30" s="18" t="s">
+      <c r="J30" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="K30" s="18"/>
+      <c r="K30" s="9"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
@@ -1729,18 +1730,18 @@
       <c r="C31" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="I31" s="18" t="s">
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="I31" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="J31" s="18" t="s">
+      <c r="J31" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="K31" s="18"/>
+      <c r="K31" s="9"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
@@ -1752,70 +1753,61 @@
       <c r="C32" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="I32" s="19" t="s">
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="I32" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="J32" s="19" t="s">
+      <c r="J32" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="K32" s="18"/>
+      <c r="K32" s="9"/>
     </row>
     <row r="33" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E33" s="12" t="s">
+      <c r="E33" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="18"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
     </row>
     <row r="34" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E34" s="11" t="s">
+      <c r="E34" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="18"/>
-      <c r="K34" s="18"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
     </row>
     <row r="35" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E35" s="9" t="s">
+      <c r="E35" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="I35" s="18"/>
-      <c r="J35" s="18"/>
-      <c r="K35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
     </row>
     <row r="36" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E36" s="9" t="s">
+      <c r="E36" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="I36" s="18"/>
-      <c r="J36" s="18"/>
-      <c r="K36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="E15:G15"/>
     <mergeCell ref="E36:G36"/>
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="E26:G26"/>
@@ -1828,6 +1820,15 @@
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="E30:G30"/>
     <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="E15:G15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Remove option for customer to input balance
</commit_message>
<xml_diff>
--- a/Bus_Booking/Dat_Ve_Xe_Khach.xlsx
+++ b/Bus_Booking/Dat_Ve_Xe_Khach.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Online\Database Management System\TH\Git\Dat_Ve_Xe_Khach\Bus_Booking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7128FC5A-89EC-4F70-A823-617511DC1A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E796353-5B18-4CE1-BB2B-0130D8073B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8C09623A-A02A-4DFB-923B-F792C92F998F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="107">
   <si>
     <t>Hệ Thống Đặt Vé Xe Khách Online</t>
   </si>
@@ -160,9 +160,6 @@
   </si>
   <si>
     <t>Khóa ngoại đặt vé (id), auto_increment.</t>
-  </si>
-  <si>
-    <t>t_tt (Tiền khách thanh toán)</t>
   </si>
   <si>
     <t>giamgia_tt (Giảm giá theo %)</t>
@@ -679,7 +676,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -723,7 +720,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1040,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D450399C-C52B-41A2-A5C9-190C77CE57CD}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F15" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1078,17 +1074,17 @@
     </row>
     <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
       <c r="E2" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="I2" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J2" s="14"/>
       <c r="K2" s="14"/>
@@ -1192,7 +1188,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>14</v>
@@ -1252,7 +1248,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>17</v>
@@ -1276,16 +1272,16 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>18</v>
@@ -1297,52 +1293,52 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L10" s="6"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I11" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K11" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="L11" s="6"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="K12" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="L12" s="6"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I13" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>19</v>
@@ -1368,17 +1364,17 @@
     </row>
     <row r="15" spans="1:12" ht="21" x14ac:dyDescent="0.4">
       <c r="A15" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="E15" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
       <c r="I15" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J15" s="16"/>
       <c r="K15" s="17"/>
@@ -1464,7 +1460,7 @@
         <v>41</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>30</v>
@@ -1488,13 +1484,13 @@
         <v>42</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>36</v>
@@ -1512,19 +1508,19 @@
         <v>30</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="F20" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>76</v>
+        <v>9</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J20" s="8" t="s">
         <v>30</v>
@@ -1542,16 +1538,7 @@
         <v>30</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="L21" s="6"/>
     </row>
@@ -1586,17 +1573,17 @@
     </row>
     <row r="25" spans="1:12" ht="21" x14ac:dyDescent="0.4">
       <c r="A25" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
       <c r="E25" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
       <c r="I25" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
@@ -1612,23 +1599,23 @@
         <v>5</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
       <c r="I26" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="J26" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="J26" s="11" t="s">
-        <v>93</v>
-      </c>
       <c r="K26" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>7</v>
@@ -1637,23 +1624,23 @@
         <v>8</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F27" s="19"/>
       <c r="G27" s="19"/>
       <c r="I27" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K27" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>30</v>
@@ -1662,90 +1649,90 @@
         <v>9</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F28" s="19"/>
       <c r="G28" s="19"/>
       <c r="I28" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K28" s="9"/>
     </row>
     <row r="29" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F29" s="19"/>
       <c r="G29" s="19"/>
       <c r="I29" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J29" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K29" s="9"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F30" s="19"/>
       <c r="G30" s="19"/>
       <c r="I30" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K30" s="9"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E31" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F31" s="19"/>
       <c r="G31" s="19"/>
       <c r="I31" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J31" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K31" s="9"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>30</v>
@@ -1754,21 +1741,21 @@
         <v>9</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F32" s="19"/>
       <c r="G32" s="19"/>
-      <c r="I32" s="21" t="s">
-        <v>107</v>
+      <c r="I32" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K32" s="9"/>
     </row>
     <row r="33" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E33" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F33" s="20"/>
       <c r="G33" s="20"/>
@@ -1778,7 +1765,7 @@
     </row>
     <row r="34" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E34" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F34" s="19"/>
       <c r="G34" s="19"/>
@@ -1788,7 +1775,7 @@
     </row>
     <row r="35" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E35" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F35" s="18"/>
       <c r="G35" s="18"/>
@@ -1798,7 +1785,7 @@
     </row>
     <row r="36" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E36" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F36" s="18"/>
       <c r="G36" s="18"/>

</xml_diff>

<commit_message>
Add changes to Excel and MySQL
</commit_message>
<xml_diff>
--- a/Bus_Booking/Dat_Ve_Xe_Khach.xlsx
+++ b/Bus_Booking/Dat_Ve_Xe_Khach.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Online\Database Management System\TH\Git\Dat_Ve_Xe_Khach\Bus_Booking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aile\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E796353-5B18-4CE1-BB2B-0130D8073B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C8D1B9-FAEB-4320-83C8-0ABC6FAD4C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8C09623A-A02A-4DFB-923B-F792C92F998F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="111">
   <si>
     <t>Hệ Thống Đặt Vé Xe Khách Online</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>Khóa ngoại đặt vé (id), auto_increment.</t>
+  </si>
+  <si>
+    <t>t_tt (Tiền khách thanh toán)</t>
   </si>
   <si>
     <t>giamgia_tt (Giảm giá theo %)</t>
@@ -251,22 +254,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Lich_Trinh (Lịch Trình) </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*****</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Dat_Ve (Đặt Vé) </t>
     </r>
     <r>
@@ -446,6 +433,44 @@
   </si>
   <si>
     <t>Thống kê doanh thu hàng tháng theo năm</t>
+  </si>
+  <si>
+    <t>id_cnlt</t>
+  </si>
+  <si>
+    <t>cn_lt</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ChoNgoi_LichTrinh (Chỗ ngồi lịch trình) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*****(2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lich_Trinh (Lịch Trình) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*****(1)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1034,17 +1059,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D450399C-C52B-41A2-A5C9-190C77CE57CD}">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.21875" customWidth="1"/>
     <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="3" max="3" width="33.77734375" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" customWidth="1"/>
     <col min="4" max="4" width="3.77734375" customWidth="1"/>
     <col min="5" max="5" width="39.21875" customWidth="1"/>
     <col min="6" max="6" width="19.77734375" customWidth="1"/>
@@ -1074,7 +1099,7 @@
     </row>
     <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -1084,7 +1109,7 @@
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="I2" s="14" t="s">
-        <v>54</v>
+        <v>110</v>
       </c>
       <c r="J2" s="14"/>
       <c r="K2" s="14"/>
@@ -1364,7 +1389,7 @@
     </row>
     <row r="15" spans="1:12" ht="21" x14ac:dyDescent="0.4">
       <c r="A15" s="14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
@@ -1374,7 +1399,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
       <c r="I15" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J15" s="16"/>
       <c r="K15" s="17"/>
@@ -1484,13 +1509,13 @@
         <v>42</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>75</v>
+        <v>9</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>36</v>
@@ -1511,13 +1536,13 @@
         <v>76</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>70</v>
@@ -1539,6 +1564,15 @@
       </c>
       <c r="C21" s="1" t="s">
         <v>73</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="L21" s="6"/>
     </row>
@@ -1573,7 +1607,7 @@
     </row>
     <row r="25" spans="1:12" ht="21" x14ac:dyDescent="0.4">
       <c r="A25" s="14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
@@ -1615,7 +1649,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>7</v>
@@ -1640,7 +1674,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>30</v>
@@ -1663,7 +1697,7 @@
     </row>
     <row r="29" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>36</v>
@@ -1686,7 +1720,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>30</v>
@@ -1709,7 +1743,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>30</v>
@@ -1732,7 +1766,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>30</v>
@@ -1753,7 +1787,7 @@
       </c>
       <c r="K32" s="9"/>
     </row>
-    <row r="33" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E33" s="20" t="s">
         <v>86</v>
       </c>
@@ -1763,7 +1797,12 @@
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
     </row>
-    <row r="34" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+      <c r="A34" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
       <c r="E34" s="19" t="s">
         <v>87</v>
       </c>
@@ -1773,7 +1812,16 @@
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
     </row>
-    <row r="35" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="E35" s="18" t="s">
         <v>88</v>
       </c>
@@ -1783,7 +1831,16 @@
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
     </row>
-    <row r="36" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="E36" s="18" t="s">
         <v>89</v>
       </c>
@@ -1793,8 +1850,30 @@
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
     </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="22">
     <mergeCell ref="E36:G36"/>
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="E26:G26"/>
@@ -1807,6 +1886,7 @@
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="E30:G30"/>
     <mergeCell ref="E34:G34"/>
+    <mergeCell ref="A34:C34"/>
     <mergeCell ref="E25:G25"/>
     <mergeCell ref="I25:K25"/>
     <mergeCell ref="A1:K1"/>

</xml_diff>